<commit_message>
Rename rate columns in APT to include _lbsacre suffix
</commit_message>
<xml_diff>
--- a/pwctool/data/Default_APT.xlsx
+++ b/pwctool/data/Default_APT.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PWC-Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PWC-Prep-Tool\pwctool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F54581-E817-4BF0-B24D-4B00E10D2C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C4D63F-FF1F-4C9F-AB4C-218ABB1C9639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="4860" windowWidth="30375" windowHeight="15750" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
+    <workbookView xWindow="780" yWindow="2625" windowWidth="24240" windowHeight="18045" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Census Naming Conv." sheetId="25" r:id="rId1"/>
+    <sheet name="Default" sheetId="25" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -68,9 +68,6 @@
     <t>MaxAnnNumApps</t>
   </si>
   <si>
-    <t>MaxAnnAmt</t>
-  </si>
-  <si>
     <t>PHI</t>
   </si>
   <si>
@@ -83,21 +80,12 @@
     <t>DriftProfile</t>
   </si>
   <si>
-    <t>PreEmergence_MaxAmt</t>
-  </si>
-  <si>
     <t>PreEmergence_MaxNumApps</t>
   </si>
   <si>
-    <t>PostEmergence_MaxAmt</t>
-  </si>
-  <si>
     <t>PostEmergence_MaxNumApps</t>
   </si>
   <si>
-    <t>Rate1_MaxAppRate</t>
-  </si>
-  <si>
     <t>Rate1_MaxNumApps</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>Rate1_Instructions</t>
   </si>
   <si>
-    <t>Rate2_MaxAppRate</t>
-  </si>
-  <si>
     <t>Rate2_MaxNumApps</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>Rate2_Instructions</t>
   </si>
   <si>
-    <t>Rate3_MaxAppRate</t>
-  </si>
-  <si>
     <t>Rate3_MaxNumApps</t>
   </si>
   <si>
@@ -140,9 +122,6 @@
     <t>Rate3_Instructions</t>
   </si>
   <si>
-    <t>Rate4_MaxAppRate</t>
-  </si>
-  <si>
     <t>Rate4_MaxNumApps</t>
   </si>
   <si>
@@ -435,6 +414,27 @@
   </si>
   <si>
     <t>Alfalfa_a</t>
+  </si>
+  <si>
+    <t>MaxAnnAmt_lbsacre</t>
+  </si>
+  <si>
+    <t>PreEmergence_MaxAmt_lbsacre</t>
+  </si>
+  <si>
+    <t>PostEmergence_MaxAmt_lbsacre</t>
+  </si>
+  <si>
+    <t>Rate1_MaxAppRate_lbsacre</t>
+  </si>
+  <si>
+    <t>Rate2_MaxAppRate_lbsacre</t>
+  </si>
+  <si>
+    <t>Rate3_MaxAppRate_lbsacre</t>
+  </si>
+  <si>
+    <t>Rate4_MaxAppRate_lbsacre</t>
   </si>
 </sst>
 </file>
@@ -915,7 +915,7 @@
   <dimension ref="A1:AH46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -926,27 +926,28 @@
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="6"/>
     <col min="9" max="9" width="5.85546875" style="18" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="5" customWidth="1"/>
     <col min="11" max="11" width="14" style="5" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="5" customWidth="1"/>
     <col min="13" max="13" width="13.5703125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="5" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" style="5" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" style="5" customWidth="1"/>
     <col min="17" max="17" width="10" style="5" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" style="18" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="5" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" style="5" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" style="5" customWidth="1"/>
     <col min="21" max="22" width="9.7109375" style="5" customWidth="1"/>
     <col min="23" max="23" width="16" style="18" customWidth="1"/>
-    <col min="24" max="25" width="10.42578125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="5" customWidth="1"/>
     <col min="26" max="26" width="9.7109375" style="5" customWidth="1"/>
     <col min="27" max="27" width="9.85546875" style="5" customWidth="1"/>
     <col min="28" max="28" width="16.28515625" style="18" customWidth="1"/>
-    <col min="29" max="29" width="9.85546875" style="5" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" style="5" customWidth="1"/>
     <col min="30" max="31" width="9.7109375" style="5" customWidth="1"/>
     <col min="32" max="32" width="10" style="5" customWidth="1"/>
     <col min="33" max="33" width="16.7109375" style="18" customWidth="1"/>
@@ -956,126 +957,126 @@
   <sheetData>
     <row r="1" spans="1:34" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AH1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C2" s="6">
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G2" s="7">
         <v>13</v>
@@ -1123,22 +1124,22 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G3" s="7">
         <v>5.4</v>
@@ -1187,22 +1188,22 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G4" s="7">
         <v>8.1</v>
@@ -1251,22 +1252,22 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C5" s="6">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G5" s="9">
         <v>2.25</v>
@@ -1296,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="S5" s="6">
         <v>0.45</v>
@@ -1307,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
@@ -1320,27 +1321,27 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="8"/>
       <c r="AH5" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G6" s="7">
         <v>4.5</v>
@@ -1370,7 +1371,7 @@
         <v>5</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="S6" s="6">
         <v>0.45</v>
@@ -1381,7 +1382,7 @@
         <v>5</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
@@ -1394,27 +1395,27 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="8"/>
       <c r="AH6" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G7" s="9">
         <v>1.35</v>
@@ -1462,22 +1463,22 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G8" s="9">
         <v>1.35</v>
@@ -1525,22 +1526,22 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G9" s="7">
         <v>5.4</v>
@@ -1594,22 +1595,22 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C10" s="6">
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G10" s="7">
         <v>1.8</v>
@@ -1663,22 +1664,22 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G11" s="7">
         <v>2.7</v>
@@ -1732,22 +1733,22 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G12" s="7">
         <v>6.3</v>
@@ -1801,22 +1802,22 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G13" s="7">
         <v>3.6</v>
@@ -1864,22 +1865,22 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G14" s="7">
         <v>3.6</v>
@@ -1927,22 +1928,22 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G15" s="7">
         <v>0.9</v>
@@ -1990,22 +1991,22 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C16" s="6">
         <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G16" s="9">
         <v>1.35</v>
@@ -2053,22 +2054,22 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C17" s="6">
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G17" s="7">
         <v>2.7</v>
@@ -2116,22 +2117,22 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G18" s="9">
         <v>2.25</v>
@@ -2179,22 +2180,22 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G19" s="7">
         <v>13</v>
@@ -2242,22 +2243,22 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G20" s="7">
         <v>13</v>
@@ -2305,22 +2306,22 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C21" s="6">
         <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G21" s="7">
         <v>1.8</v>
@@ -2368,22 +2369,22 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C22" s="6">
         <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G22" s="7">
         <v>4.5</v>
@@ -2431,22 +2432,22 @@
     </row>
     <row r="23" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C23" s="12">
         <v>2</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G23" s="13">
         <v>0.9</v>
@@ -2494,22 +2495,22 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C24" s="6">
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G24" s="7">
         <v>13</v>
@@ -2557,22 +2558,22 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C25" s="6">
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G25" s="7">
         <v>5.4</v>
@@ -2621,22 +2622,22 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C26" s="6">
         <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G26" s="7">
         <v>8.1</v>
@@ -2685,22 +2686,22 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C27" s="6">
         <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G27" s="9">
         <v>2.25</v>
@@ -2730,7 +2731,7 @@
         <v>5</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="S27" s="6">
         <v>0.45</v>
@@ -2741,7 +2742,7 @@
         <v>5</v>
       </c>
       <c r="W27" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="X27" s="6"/>
       <c r="Y27" s="6"/>
@@ -2754,27 +2755,27 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="8"/>
       <c r="AH27" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C28" s="6">
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G28" s="7">
         <v>4.5</v>
@@ -2804,7 +2805,7 @@
         <v>5</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="S28" s="6">
         <v>0.45</v>
@@ -2815,7 +2816,7 @@
         <v>5</v>
       </c>
       <c r="W28" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="X28" s="6"/>
       <c r="Y28" s="6"/>
@@ -2828,27 +2829,27 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="8"/>
       <c r="AH28" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C29" s="6">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G29" s="9">
         <v>1.35</v>
@@ -2896,22 +2897,22 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C30" s="6">
         <v>2</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G30" s="9">
         <v>1.35</v>
@@ -2959,22 +2960,22 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G31" s="7">
         <v>5.4</v>
@@ -3028,22 +3029,22 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C32" s="6">
         <v>2</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G32" s="7">
         <v>1.8</v>
@@ -3097,22 +3098,22 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C33" s="6">
         <v>2</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G33" s="7">
         <v>2.7</v>
@@ -3166,22 +3167,22 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C34" s="6">
         <v>2</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G34" s="7">
         <v>6.3</v>
@@ -3235,22 +3236,22 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C35" s="6">
         <v>2</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G35" s="7">
         <v>3.6</v>
@@ -3298,22 +3299,22 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C36" s="6">
         <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G36" s="7">
         <v>3.6</v>
@@ -3361,22 +3362,22 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C37" s="6">
         <v>2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G37" s="7">
         <v>0.9</v>
@@ -3424,22 +3425,22 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C38" s="6">
         <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G38" s="9">
         <v>1.35</v>
@@ -3487,22 +3488,22 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C39" s="6">
         <v>2</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G39" s="7">
         <v>2.7</v>
@@ -3550,22 +3551,22 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C40" s="6">
         <v>2</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G40" s="9">
         <v>2.25</v>
@@ -3613,22 +3614,22 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C41" s="6">
         <v>2</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G41" s="7">
         <v>13</v>
@@ -3676,22 +3677,22 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C42" s="6">
         <v>2</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G42" s="7">
         <v>13</v>
@@ -3739,22 +3740,22 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C43" s="6">
         <v>2</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G43" s="7">
         <v>1.8</v>
@@ -3802,22 +3803,22 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C44" s="6">
         <v>2</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G44" s="7">
         <v>4.5</v>
@@ -3865,22 +3866,22 @@
     </row>
     <row r="45" spans="1:33" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C45" s="12">
         <v>2</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G45" s="13">
         <v>0.9</v>
@@ -3928,22 +3929,22 @@
     </row>
     <row r="46" spans="1:33" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="C46" s="16">
         <v>1</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G46" s="15">
         <v>1.5</v>
@@ -3973,12 +3974,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bbec734e-c9c2-4352-b3fc-6a37619c639c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="45003b2f-0c5d-4c18-a036-4ca6f26534cb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4207,20 +4210,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bbec734e-c9c2-4352-b3fc-6a37619c639c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="45003b2f-0c5d-4c18-a036-4ca6f26534cb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
+    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4245,18 +4255,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
-    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>